<commit_message>
Add MVP for test package
</commit_message>
<xml_diff>
--- a/internal/tg/File/MatLab/10/tim.xlsx
+++ b/internal/tg/File/MatLab/10/tim.xlsx
@@ -45317,96 +45317,6 @@
         <v>299.96666666668966</v>
       </c>
     </row>
-    <row r="9001">
-      <c r="A9001">
-        <v>300.000000000023</v>
-      </c>
-    </row>
-    <row r="9002">
-      <c r="A9002">
-        <v>300.0333333333564</v>
-      </c>
-    </row>
-    <row r="9003">
-      <c r="A9003">
-        <v>300.06666666668974</v>
-      </c>
-    </row>
-    <row r="9004">
-      <c r="A9004">
-        <v>300.1000000000231</v>
-      </c>
-    </row>
-    <row r="9005">
-      <c r="A9005">
-        <v>300.13333333335646</v>
-      </c>
-    </row>
-    <row r="9006">
-      <c r="A9006">
-        <v>300.1666666666898</v>
-      </c>
-    </row>
-    <row r="9007">
-      <c r="A9007">
-        <v>300.2000000000232</v>
-      </c>
-    </row>
-    <row r="9008">
-      <c r="A9008">
-        <v>300.23333333335654</v>
-      </c>
-    </row>
-    <row r="9009">
-      <c r="A9009">
-        <v>300.2666666666899</v>
-      </c>
-    </row>
-    <row r="9010">
-      <c r="A9010">
-        <v>300.30000000002326</v>
-      </c>
-    </row>
-    <row r="9011">
-      <c r="A9011">
-        <v>300.3333333333566</v>
-      </c>
-    </row>
-    <row r="9012">
-      <c r="A9012">
-        <v>300.36666666669</v>
-      </c>
-    </row>
-    <row r="9013">
-      <c r="A9013">
-        <v>300.40000000002334</v>
-      </c>
-    </row>
-    <row r="9014">
-      <c r="A9014">
-        <v>300.4333333333567</v>
-      </c>
-    </row>
-    <row r="9015">
-      <c r="A9015">
-        <v>300.46666666669006</v>
-      </c>
-    </row>
-    <row r="9016">
-      <c r="A9016">
-        <v>300.5000000000234</v>
-      </c>
-    </row>
-    <row r="9017">
-      <c r="A9017">
-        <v>300.5333333333568</v>
-      </c>
-    </row>
-    <row r="9018">
-      <c r="A9018">
-        <v>300.56666666669014</v>
-      </c>
-    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>